<commit_message>
added sangeet1 - first 2 rows
</commit_message>
<xml_diff>
--- a/testGIT1.xlsx
+++ b/testGIT1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\GitTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A778A8E6-E58E-46E6-85FF-A62942B0158A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510EF5C-886C-476E-8448-7FA02B545651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VersionHistory" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -212,6 +212,9 @@
   <si>
     <t>left outer join
 analytics_study_metrics.study=analytics_study_milestones_metrics.study_name</t>
+  </si>
+  <si>
+    <t>sangeet1</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -676,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A7D3C7-9356-4524-BFF4-AE95A7867A08}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,7 +735,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -752,7 +755,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>

</xml_diff>

<commit_message>
simulate a merge - step 1 - changed by sangeetkhullar that is cloned by sangeetDSI
</commit_message>
<xml_diff>
--- a/testGIT1.xlsx
+++ b/testGIT1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\GitTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63259597-92EE-467F-A3E1-95BCA0DE0EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB39CBD3-03C8-49E1-A402-BB97596966FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>sangeet2</t>
+  </si>
+  <si>
+    <t>sangeet3</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,7 +823,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -840,7 +843,7 @@
         <v>46</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>

</xml_diff>

<commit_message>
2nd user changed the same cell - should create merge conflict
</commit_message>
<xml_diff>
--- a/testGIT1.xlsx
+++ b/testGIT1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\GitTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\GitMergeSimulation\excel_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63259597-92EE-467F-A3E1-95BCA0DE0EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E851CBA7-4DB1-44D3-A1F7-592BCA936E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VersionHistory" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>sangeet2</t>
+  </si>
+  <si>
+    <t>merge simulation - changed same cell</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,7 +823,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -840,7 +843,7 @@
         <v>46</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>

</xml_diff>